<commit_message>
Updated latest Guinea master data.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/app_detail.xlsx
+++ b/mosip_master/xlsx/app_detail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wuriguineecom-my.sharepoint.com/personal/iteli_bah_wuriguinee_com/Documents/Bureau/master-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Mosip Codebase\GUINEA_Pilot\GUINEA_Pilot_Mosip-Data_WuriGuinea-1.2.0.1-B1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{777852F3-C7AE-4597-87F9-4151CCDA3985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4341B70-1391-4E97-AF74-3DD3E59D3AB8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D987F12E-0BCF-4B12-A634-F282B02CB743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9875" yWindow="45" windowWidth="9330" windowHeight="9400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -37,18 +37,9 @@
     <t>is_active</t>
   </si>
   <si>
-    <t>Pré-Enregistrement</t>
-  </si>
-  <si>
-    <t>Portail Web pour les pré-enregistrements</t>
-  </si>
-  <si>
     <t>fra</t>
   </si>
   <si>
-    <t>TRUE</t>
-  </si>
-  <si>
     <t>Enregistrement</t>
   </si>
   <si>
@@ -73,10 +64,40 @@
     <t>Portail Web pour la configuration des applications</t>
   </si>
   <si>
-    <t>Portail Résident</t>
-  </si>
-  <si>
-    <t>Portail Web pour les services dédiés aux résidents</t>
+    <t>cr_by</t>
+  </si>
+  <si>
+    <t>cr_dtimes</t>
+  </si>
+  <si>
+    <t>upd_by</t>
+  </si>
+  <si>
+    <t>upd_dtimes</t>
+  </si>
+  <si>
+    <t>is_deleted</t>
+  </si>
+  <si>
+    <t>del_dtimes</t>
+  </si>
+  <si>
+    <t>PrÃ©-Enregistrement</t>
+  </si>
+  <si>
+    <t>Portail Web pour les prÃ©-enregistrements</t>
+  </si>
+  <si>
+    <t>superadmin</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Portail RÃ©sident</t>
+  </si>
+  <si>
+    <t>Portail Web pour les services dÃ©diÃ©s aux rÃ©sidents</t>
   </si>
 </sst>
 </file>
@@ -568,53 +589,54 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -630,7 +652,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -926,136 +948,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>10001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45079.576688067129</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>10003</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>10001</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45079.576688067129</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>10005</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1">
+        <v>45079.576688067129</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>10003</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>10007</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45079.576688067129</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>10005</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>10009</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45079.576688067129</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>10007</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>10009</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>10011</v>
       </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45079.576688067129</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>